<commit_message>
Updated BOM with test points
</commit_message>
<xml_diff>
--- a/Accessories/ExpansionBoard_DAC/REV20200720B/DAC_bom_qty_1.xlsx
+++ b/Accessories/ExpansionBoard_DAC/REV20200720B/DAC_bom_qty_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandt\Documents\AMDC-Hardware\Accessories\ExpansionBoard_DAC\REV20200627B\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandt\Documents\AMDC-Hardware\Accessories\ExpansionBoard_DAC\REV20200720B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFE59A5-C9C6-4333-A8C5-15E24C41AEF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60687B29-2C6A-4713-BE1D-176C29955A02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0E5B20F1-3507-443B-9CC0-A247604A0E71}"/>
+    <workbookView xWindow="3720" yWindow="2355" windowWidth="21600" windowHeight="11385" xr2:uid="{A38E6318-F650-4269-8D5C-2DA282BB5A95}"/>
   </bookViews>
   <sheets>
     <sheet name="DAC_bom_qty_1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
   <si>
     <t>Quantity</t>
   </si>
@@ -279,6 +279,15 @@
   </si>
   <si>
     <t>HX1188NLT</t>
+  </si>
+  <si>
+    <t>A106145CT-ND</t>
+  </si>
+  <si>
+    <t>TP1, TP2, TP3, TP4, TP5</t>
+  </si>
+  <si>
+    <t>Test Point</t>
   </si>
   <si>
     <t>ADUM130E1BRWZ-ND</t>
@@ -750,13 +759,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8BA961-F042-4B17-A8EF-23D76334F1B3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D47BA9C9-50A2-4AFE-B58E-CD0AC8FF89EA}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
@@ -1190,7 +1199,7 @@
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>81</v>
@@ -1203,7 +1212,7 @@
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1224,9 +1233,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>87</v>
@@ -1239,7 +1248,7 @@
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1262,7 +1271,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>93</v>
@@ -1275,10 +1284,10 @@
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>1</v>
       </c>
@@ -1314,7 +1323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>1</v>
       </c>
@@ -1332,7 +1341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>1</v>
       </c>
@@ -1365,12 +1374,30 @@
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>1</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup scale="52" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
+  <pageSetup scale="50" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>